<commit_message>
Added sempahore to ISR for IR reading + continious and discreet IR control Defined buttons Added Stub for USB tests Added cancel_callback for ISRs in timers ADDED LCD LOGIC :D (under effects.h)
</commit_message>
<xml_diff>
--- a/adc_transformation.xlsx
+++ b/adc_transformation.xlsx
@@ -159,23 +159,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="60058240"/>
-        <c:axId val="60056704"/>
+        <c:axId val="117182848"/>
+        <c:axId val="117184384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60058240"/>
+        <c:axId val="117182848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60056704"/>
+        <c:crossAx val="117184384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60056704"/>
+        <c:axId val="117184384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -183,7 +183,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60058240"/>
+        <c:crossAx val="117182848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -196,7 +196,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -256,54 +256,54 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.4444444444444446</c:v>
+                  <c:v>35.555555555555557</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.7419354838709671</c:v>
+                  <c:v>61.935483870967737</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5238095238095237</c:v>
+                  <c:v>76.19047619047619</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.320754716981131</c:v>
+                  <c:v>90.566037735849051</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.903225806451614</c:v>
+                  <c:v>103.22580645161291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.46153846153846</c:v>
+                  <c:v>147.69230769230768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="103876480"/>
-        <c:axId val="103874944"/>
+        <c:axId val="117212288"/>
+        <c:axId val="117213824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103876480"/>
+        <c:axId val="117212288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103874944"/>
+        <c:crossAx val="117213824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103874944"/>
+        <c:axId val="117213824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -311,7 +311,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103876480"/>
+        <c:crossAx val="117212288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -324,7 +324,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -683,7 +683,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -718,8 +718,8 @@
         <v>230.4</v>
       </c>
       <c r="D3">
-        <f>1024/C3</f>
-        <v>4.4444444444444446</v>
+        <f>8*1024/C3</f>
+        <v>35.555555555555557</v>
       </c>
       <c r="E3">
         <f>(C3+C4)/2</f>
@@ -738,8 +738,8 @@
         <v>170.66666666666666</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D11" si="1">1024/C4</f>
-        <v>6</v>
+        <f t="shared" ref="D4:D11" si="1">8*1024/C4</f>
+        <v>48</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E10" si="2">(C4+C5)/2</f>
@@ -759,7 +759,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>7.7419354838709671</v>
+        <v>61.935483870967737</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
@@ -779,7 +779,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>9.5238095238095237</v>
+        <v>76.19047619047619</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
@@ -799,7 +799,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>11.320754716981131</v>
+        <v>90.566037735849051</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
@@ -819,7 +819,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>12.903225806451614</v>
+        <v>103.22580645161291</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
@@ -839,7 +839,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
@@ -859,7 +859,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
@@ -879,7 +879,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>18.46153846153846</v>
+        <v>147.69230769230768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>